<commit_message>
[fixes] - clarify error message when screenshot cannot be taken
[desktop]
- ensure Winium driver and `notifu.exe` are not executed in non-Windows environment.
- [`typeKeys(os,keystrokes)`]: support UPPERCASE typing.
- [`typeKeys(os,keystrokes)`]: support non-alphanumeric symbol typing.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_web.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_web.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0B066C-6509-9541-9C2E-751A47F95219}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75BFC6E-1444-7F41-82B2-3B768C08A837}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15760" tabRatio="420" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15760" tabRatio="420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <sheet name="SavePartialText" sheetId="20" r:id="rId14"/>
     <sheet name="DoubleClick" sheetId="22" r:id="rId15"/>
     <sheet name="MouseOver" sheetId="23" r:id="rId16"/>
-    <sheet name="AssertTypeKeys" sheetId="24" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
@@ -82,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="766">
   <si>
     <t>target</t>
   </si>
@@ -2392,73 +2391,17 @@
   <si>
     <t>spellCheck(var,profile,text)</t>
   </si>
-  <si>
-    <t>testing the use of desktop.typeKeys() on web page</t>
-  </si>
-  <si>
-    <t>open site</t>
-  </si>
-  <si>
-    <t>https://www.quackit.com/html_5/tags/html_textarea_tag.cfm</t>
-  </si>
-  <si>
-    <t>name=result1</t>
-  </si>
-  <si>
-    <t>css=textarea</t>
-  </si>
-  <si>
-    <t>css=.submit</t>
-  </si>
-  <si>
-    <t>focus on textarea</t>
-  </si>
-  <si>
-    <t>Mac,Windows</t>
-  </si>
-  <si>
-    <t>reset textarea for bigger editor</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>`~!@#$%^&amp;*()-_=+[]{}\|;:'",./&lt;&gt;?</t>
-  </si>
-  <si>
-    <t>type keys</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>[]\{}| ;':" ,./&lt;&gt;? ~!@#$%^&amp;*()_+ `1234567890-=</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2660,102 +2603,102 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2766,38 +2709,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2809,11 +2743,11 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2821,7 +2755,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2833,7 +2767,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2845,49 +2779,13 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="102">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="99">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -6111,12 +6009,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -6133,20 +6031,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -6155,10 +6053,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -6675,13 +6573,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="26" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="23" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="25" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="22" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="21" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6725,12 +6623,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -6747,20 +6645,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -6769,10 +6667,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -7066,13 +6964,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="23" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="20" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="19" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="18" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7116,12 +7014,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -7138,20 +7036,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -7160,10 +7058,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -7326,13 +7224,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="20" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="17" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="16" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="15" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7377,12 +7275,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -7399,20 +7297,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -7421,10 +7319,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -7710,13 +7608,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="17" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="14" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="13" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="15" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="12" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7761,12 +7659,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -7783,20 +7681,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -7805,10 +7703,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -8027,13 +7925,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="9" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8079,12 +7977,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -8101,20 +7999,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -8123,10 +8021,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -8598,24 +8496,24 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N10:N11">
-    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="8" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N10,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="7" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N10,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="6" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N10,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1 N3:N9 N12:N1048576">
-    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="5" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="4" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="3" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8662,12 +8560,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -8684,20 +8582,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -8706,10 +8604,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -8920,13 +8818,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="5" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="2" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="0" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8945,1161 +8843,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10C8890-277D-144D-B477-FA86229E725D}">
-  <dimension ref="A1:O67"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.83203125" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.83203125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="41" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="10" width="30" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="1.6640625" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" style="7" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.5" style="8" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.83203125" style="7" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="49.83203125" style="6" customWidth="1" collapsed="1"/>
-    <col min="16" max="16384" width="10.83203125" style="9" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>348</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>615</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>616</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
-        <v>352</v>
-      </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
-    </row>
-    <row r="2" spans="1:15" ht="133" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>766</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12" t="s">
-        <v>604</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
-    </row>
-    <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="8"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="19"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>767</v>
-      </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>768</v>
-      </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-    </row>
-    <row r="6" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>619</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>774</v>
-      </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-    </row>
-    <row r="7" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>771</v>
-      </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-    </row>
-    <row r="8" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>772</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>769</v>
-      </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-    </row>
-    <row r="9" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>770</v>
-      </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-    </row>
-    <row r="10" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>775</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-    </row>
-    <row r="11" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>777</v>
-      </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>753</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>773</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>779</v>
-      </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-    </row>
-    <row r="12" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>770</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>778</v>
-      </c>
-      <c r="G12" s="55" t="s">
-        <v>779</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="6"/>
-    </row>
-    <row r="15" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="6"/>
-    </row>
-    <row r="16" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="54" t="s">
-        <v>776</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="6"/>
-    </row>
-    <row r="18" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="6"/>
-    </row>
-    <row r="19" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="6"/>
-    </row>
-    <row r="20" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="6"/>
-    </row>
-    <row r="21" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="6"/>
-    </row>
-    <row r="22" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="6"/>
-    </row>
-    <row r="23" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="6"/>
-    </row>
-    <row r="24" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="6"/>
-    </row>
-    <row r="25" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="6"/>
-    </row>
-    <row r="26" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="6"/>
-    </row>
-    <row r="27" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="6"/>
-    </row>
-    <row r="28" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="6"/>
-    </row>
-    <row r="29" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="6"/>
-    </row>
-    <row r="30" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="6"/>
-    </row>
-    <row r="31" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="6"/>
-    </row>
-    <row r="32" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="6"/>
-    </row>
-    <row r="33" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="6"/>
-    </row>
-    <row r="34" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="6"/>
-    </row>
-    <row r="35" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="6"/>
-    </row>
-    <row r="36" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="6"/>
-    </row>
-    <row r="37" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="6"/>
-    </row>
-    <row r="38" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="6"/>
-    </row>
-    <row r="39" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="6"/>
-    </row>
-    <row r="40" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="6"/>
-    </row>
-    <row r="41" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="6"/>
-    </row>
-    <row r="42" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="6"/>
-    </row>
-    <row r="43" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="6"/>
-    </row>
-    <row r="44" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="6"/>
-    </row>
-    <row r="45" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="6"/>
-    </row>
-    <row r="46" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="6"/>
-    </row>
-    <row r="47" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="6"/>
-    </row>
-    <row r="48" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="6"/>
-    </row>
-    <row r="49" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="6"/>
-    </row>
-    <row r="50" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="6"/>
-    </row>
-    <row r="51" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="6"/>
-    </row>
-    <row r="52" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="6"/>
-    </row>
-    <row r="53" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="6"/>
-    </row>
-    <row r="54" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="6"/>
-    </row>
-    <row r="55" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="6"/>
-    </row>
-    <row r="56" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="7"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="6"/>
-    </row>
-    <row r="57" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="6"/>
-    </row>
-    <row r="58" spans="1:15" s="34" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="6"/>
-    </row>
-    <row r="59" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="L2:O2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
-      <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
-      <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
-      <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D54" xr:uid="{BC54E1D9-6B32-EB45-B386-318ABEC45F7B}">
-      <formula1>INDIRECT(C5)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C11" xr:uid="{D4A67003-E54D-B240-823A-9D6D6B45B197}">
-      <formula1>target</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" tooltip="http://money.cnn.com/" display="http://money.cnn.com/" xr:uid="{8F452757-CBAC-E64E-8494-4DA1D36FB412}"/>
-  </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
@@ -10120,12 +8868,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -10142,20 +8890,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>353</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="27"/>
       <c r="G2" s="11"/>
@@ -10164,10 +8912,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -10443,13 +9191,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="101" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="98" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="100" priority="13" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="97" priority="13" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="99" priority="15" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="96" priority="15" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10493,12 +9241,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -10515,20 +9263,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>353</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="27"/>
       <c r="G2" s="11"/>
@@ -10537,10 +9285,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -11707,13 +10455,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="98" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="95" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="97" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="94" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="93" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11763,12 +10511,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -11785,20 +10533,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>353</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="27"/>
       <c r="G2" s="11"/>
@@ -11807,10 +10555,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -12217,13 +10965,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="95" priority="13" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="92" priority="13" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="14" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="91" priority="14" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="93" priority="15" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="90" priority="15" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12270,12 +11018,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -12292,20 +11040,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="140" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>353</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="27"/>
       <c r="G2" s="11"/>
@@ -12314,10 +11062,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -12759,13 +11507,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="92" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="89" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="91" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="88" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="90" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="87" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12811,12 +11559,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -12833,20 +11581,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="27"/>
       <c r="G2" s="11"/>
@@ -12855,10 +11603,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -13643,189 +12391,189 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N8">
-    <cfRule type="beginsWith" dxfId="89" priority="58" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="86" priority="58" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N8,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="88" priority="59" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="85" priority="59" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N8,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="87" priority="60" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="84" priority="60" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N8,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="beginsWith" dxfId="86" priority="55" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="83" priority="55" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N12,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="85" priority="56" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="82" priority="56" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N12,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="84" priority="57" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="81" priority="57" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N12,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="beginsWith" dxfId="83" priority="19" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="80" priority="19" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N17,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="82" priority="20" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="79" priority="20" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N17,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="81" priority="21" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="78" priority="21" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N17,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20">
-    <cfRule type="beginsWith" dxfId="80" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="77" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N20,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="79" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="76" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N20,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="75" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N20,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21">
-    <cfRule type="beginsWith" dxfId="77" priority="43" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="74" priority="43" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N21,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="44" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="73" priority="44" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N21,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="75" priority="45" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="72" priority="45" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N21,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22">
-    <cfRule type="beginsWith" dxfId="74" priority="37" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="71" priority="37" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N22,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="73" priority="38" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="70" priority="38" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N22,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="72" priority="39" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="69" priority="39" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N22,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="beginsWith" dxfId="71" priority="13" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="68" priority="13" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N26,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="70" priority="14" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="67" priority="14" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N26,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="69" priority="15" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="66" priority="15" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N26,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="beginsWith" dxfId="68" priority="40" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="65" priority="40" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N27,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="67" priority="41" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="64" priority="41" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N27,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="66" priority="42" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="63" priority="42" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N27,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28">
-    <cfRule type="beginsWith" dxfId="65" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="62" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N28,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="64" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="61" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N28,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="63" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="60" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N28,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29">
-    <cfRule type="beginsWith" dxfId="62" priority="31" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="59" priority="31" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N29,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="61" priority="32" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="58" priority="32" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N29,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="60" priority="33" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="57" priority="33" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N29,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30">
-    <cfRule type="beginsWith" dxfId="59" priority="25" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="56" priority="25" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N30,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="26" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="55" priority="26" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N30,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="57" priority="27" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="54" priority="27" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N30,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34">
-    <cfRule type="beginsWith" dxfId="56" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="53" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N34,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="55" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="52" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N34,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="51" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N34,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13:N16">
-    <cfRule type="beginsWith" dxfId="53" priority="49" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="50" priority="49" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N13,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="52" priority="50" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="49" priority="50" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N13,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="51" priority="51" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="48" priority="51" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N13,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N19">
-    <cfRule type="beginsWith" dxfId="50" priority="52" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="47" priority="52" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N18,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="49" priority="53" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="46" priority="53" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N18,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="54" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="45" priority="54" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N18,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23:N25">
-    <cfRule type="beginsWith" dxfId="47" priority="16" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="44" priority="16" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N23,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="46" priority="17" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="43" priority="17" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N23,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="45" priority="18" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="42" priority="18" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N23,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N31:N33">
-    <cfRule type="beginsWith" dxfId="44" priority="10" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="41" priority="10" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N31,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="43" priority="11" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="40" priority="11" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N31,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="42" priority="12" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="39" priority="12" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N31,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1 N3:N7 N9:N11">
-    <cfRule type="beginsWith" dxfId="41" priority="70" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="38" priority="70" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="71" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="37" priority="71" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="39" priority="72" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="36" priority="72" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13869,12 +12617,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -13891,20 +12639,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -13913,10 +12661,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -14363,24 +13111,24 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N10">
-    <cfRule type="beginsWith" dxfId="38" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="35" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N10,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="37" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="34" priority="5" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N10,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="33" priority="6" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N10,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1 N3:N9 N11:N1048576">
-    <cfRule type="beginsWith" dxfId="35" priority="10" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="32" priority="10" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="11" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="31" priority="11" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="33" priority="12" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="30" priority="12" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14425,12 +13173,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -14447,20 +13195,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -14469,10 +13217,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -15042,13 +13790,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N23 N35:N1048576 L24:L34">
-    <cfRule type="beginsWith" dxfId="32" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="29" priority="7" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(L1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="31" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="28" priority="8" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(L1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="30" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="27" priority="9" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(L1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15093,12 +13841,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="10" t="s">
         <v>349</v>
       </c>
@@ -15115,20 +13863,20 @@
         <v>351</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>428</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -15137,10 +13885,10 @@
         <v>604</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="8"/>
@@ -17028,13 +15776,13 @@
     <mergeCell ref="L2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="N1 N3:N1048576">
-    <cfRule type="beginsWith" dxfId="29" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
+    <cfRule type="beginsWith" dxfId="26" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="28" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
+    <cfRule type="beginsWith" dxfId="25" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
       <formula>LEFT(N1,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="27" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
+    <cfRule type="beginsWith" dxfId="24" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[improvements] - [`nexial.lastElapsedTime`]: record the elapsed time (in ms) for the last executed step (regardless of its PASS or FAIL status).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_web.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CACBF2-65C1-9E45-8828-C892348B4BCF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E036C1-ECE6-4B45-ACBF-7BE719E10206}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="31540" tabRatio="420" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14974,7 +14974,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[web] - [`saveISTDivsAsCsv`]: improved on scanning and data collection logic. Now works reliably over 500 rows of infinite   scroll table.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_web.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_web.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E036C1-ECE6-4B45-ACBF-7BE719E10206}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D9F620-E4F9-F245-B674-6DB2C531534C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="31540" tabRatio="420" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="31540" tabRatio="420" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2490,9 +2490,9 @@
   </si>
   <si>
     <t>header-cell=css=.ui-grid-header-cell-row .ui-grid-cell-contents
-data-row=css=.ui-grid-row
-data-cell=css=.ui-grid-cell-contents
 data-viewport=css=.ui-grid-viewport
+data-row-xpath=.//*[contains(@class,"ui-grid-row")]
+data-cell-xpath=.//*[contains(@class,"ui-grid-cell-contents")]
 limit=-1
 nexial.web.saveGrid.deepScan=true</t>
   </si>
@@ -14973,8 +14973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B71B0E-64AD-1949-8FC9-9915E9588508}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14983,7 +14983,7 @@
     <col min="2" max="2" width="57.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.33203125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="64.83203125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="68" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="37" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="27.6640625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="9" width="10.6640625" style="4" customWidth="1" collapsed="1"/>
@@ -15244,7 +15244,7 @@
       <c r="N9"/>
       <c r="O9"/>
     </row>
-    <row r="10" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">

</xml_diff>

<commit_message>
[improvements] - [`nexial.outputToCloud`]: now support other file-based resources so that when `nexial.outputToCloud` is set to true, file-based resources will be pushed to the Cloud automatically (and its link on the output will be updated as well.)
[ws]
- fixed: handle url that contains "percent-encoding" by avoiding double-encoding error.

[web]
- [`saveISTDivsAsCsv`]: improved on usability by allowing for configurable "waitBetweenScroll" value.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_web.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_web.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D9F620-E4F9-F245-B674-6DB2C531534C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F969DB-11C4-1F4C-BA8E-B5095F6EEA89}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="31540" tabRatio="420" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10980" windowWidth="51200" windowHeight="21020" tabRatio="420" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="810">
   <si>
     <t>target</t>
   </si>
@@ -2495,6 +2495,37 @@
 data-cell-xpath=.//*[contains(@class,"ui-grid-cell-contents")]
 limit=-1
 nexial.web.saveGrid.deepScan=true</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/table3-ist.csv</t>
+  </si>
+  <si>
+    <t>collect data from IST grid</t>
+  </si>
+  <si>
+    <t>compare against known baseline</t>
+  </si>
+  <si>
+    <t>$(syspath|out|fullpath)/table3c.csv</t>
+  </si>
+  <si>
+    <t>header-cell=css=.ui-grid-header-cell-row .ui-grid-cell-contents
+data-viewport=css=.ui-grid-viewport
+data-row-xpath=.//*[contains(@class,"ui-grid-row")]
+data-cell-xpath=.//*[contains(@class,"ui-grid-cell-contents")]
+limit=-1
+nexial.web.saveGrid.deepScan=true
+nexial.web.saveGrid.data.trim=true
+nexial.web.saveGrid.end.trim=true</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/table3-ist-a.csv</t>
+  </si>
+  <si>
+    <t>file:///$(syspath|data|fullpath)/web/ui-grid-example/example-a.html</t>
+  </si>
+  <si>
+    <t>next IST - slightly more complex (spaces and HTML)</t>
   </si>
 </sst>
 </file>
@@ -2732,7 +2763,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2950,6 +2981,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -14971,10 +15009,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B71B0E-64AD-1949-8FC9-9915E9588508}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14983,7 +15021,7 @@
     <col min="2" max="2" width="57.6640625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.33203125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="68" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="70" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="37" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="27.6640625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="9" width="10.6640625" style="4" customWidth="1" collapsed="1"/>
@@ -15115,10 +15153,9 @@
       <c r="E5" s="30" t="s">
         <v>765</v>
       </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="30"/>
+      <c r="F5" s="30" t="s">
+        <v>435</v>
+      </c>
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
       <c r="J5" s="27"/>
@@ -15141,7 +15178,7 @@
       <c r="D6" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="66" t="s">
         <v>785</v>
       </c>
       <c r="F6"/>
@@ -15230,7 +15267,7 @@
       <c r="D9" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="65" t="s">
         <v>785</v>
       </c>
       <c r="F9" s="8"/>
@@ -15246,7 +15283,9 @@
     </row>
     <row r="10" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>803</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -15270,10 +15309,24 @@
       <c r="O10"/>
     </row>
     <row r="11" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="4"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="30"/>
+      <c r="B11" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>802</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>800</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>439</v>
+      </c>
       <c r="H11" s="30"/>
       <c r="I11" s="30"/>
       <c r="J11" s="27"/>
@@ -15284,10 +15337,19 @@
       <c r="O11"/>
     </row>
     <row r="12" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="4"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="51"/>
+      <c r="B12" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E12" s="65" t="s">
+        <v>808</v>
+      </c>
+      <c r="F12" s="31"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
       <c r="I12" s="30"/>
@@ -15298,11 +15360,23 @@
       <c r="N12"/>
       <c r="O12"/>
     </row>
-    <row r="13" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
-      <c r="B13" s="4"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="31"/>
+    <row r="13" spans="1:15" ht="128" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="4" t="s">
+        <v>803</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>799</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>806</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>805</v>
+      </c>
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
@@ -15315,10 +15389,24 @@
     </row>
     <row r="14" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="46"/>
-      <c r="B14" s="4"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="30"/>
+      <c r="B14" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>807</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>805</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>439</v>
+      </c>
       <c r="H14" s="30"/>
       <c r="I14" s="30"/>
       <c r="J14" s="27"/>
@@ -15333,6 +15421,7 @@
       <c r="B15" s="4"/>
       <c r="E15" s="23"/>
       <c r="F15" s="52"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
       <c r="J15" s="27"/>
@@ -15346,8 +15435,7 @@
       <c r="A16" s="46"/>
       <c r="B16" s="4"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="27"/>
+      <c r="F16" s="52"/>
       <c r="H16" s="30"/>
       <c r="I16" s="30"/>
       <c r="J16" s="27"/>
@@ -15373,7 +15461,7 @@
       <c r="O17"/>
     </row>
     <row r="18" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="4"/>
       <c r="E18" s="23"/>
       <c r="F18" s="51"/>
@@ -15392,6 +15480,7 @@
       <c r="B19" s="4"/>
       <c r="E19" s="23"/>
       <c r="F19" s="51"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="30"/>
       <c r="I19" s="30"/>
       <c r="J19" s="27"/>
@@ -15405,7 +15494,7 @@
       <c r="A20" s="12"/>
       <c r="B20" s="4"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
+      <c r="F20" s="51"/>
       <c r="H20" s="30"/>
       <c r="I20" s="30"/>
       <c r="J20" s="27"/>
@@ -15416,11 +15505,10 @@
       <c r="O20"/>
     </row>
     <row r="21" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="46"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="4"/>
       <c r="E21" s="23"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="27"/>
+      <c r="F21" s="23"/>
       <c r="H21" s="30"/>
       <c r="I21" s="30"/>
       <c r="J21" s="27"/>
@@ -15435,7 +15523,7 @@
       <c r="B22" s="4"/>
       <c r="E22" s="23"/>
       <c r="F22" s="31"/>
-      <c r="G22" s="30"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="30"/>
       <c r="I22" s="30"/>
       <c r="J22" s="27"/>
@@ -15446,30 +15534,45 @@
       <c r="O22"/>
     </row>
     <row r="23" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="46"/>
+      <c r="B23" s="4"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="52"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="39"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
     </row>
     <row r="24" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
+      <c r="F24" s="52"/>
     </row>
     <row r="25" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
     </row>
     <row r="26" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="4"/>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
     </row>
     <row r="28" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+    </row>
     <row r="30" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
@@ -15477,7 +15580,7 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="N1 N3:N23">
+  <conditionalFormatting sqref="N1 N3:N24">
     <cfRule type="beginsWith" dxfId="29" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -15488,11 +15591,11 @@
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D25" xr:uid="{43C64BA3-34C6-E946-B752-182901936CBC}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D26" xr:uid="{43C64BA3-34C6-E946-B752-182901936CBC}">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C25" xr:uid="{EEE4BB8C-7225-C04F-967D-7548E7A06B88}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C26" xr:uid="{EEE4BB8C-7225-C04F-967D-7548E7A06B88}">
       <formula1>target</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>